<commit_message>
Added: 8DIO The New Ambient Guitar 8DIO The New Forgotten Voices Cait
Modified:
XLSX format
</commit_message>
<xml_diff>
--- a/8DIO/Claire Woodwinds/Claire Clarinet/xlsx/Claire Clarinet.xlsx
+++ b/8DIO/Claire Woodwinds/Claire Clarinet/xlsx/Claire Clarinet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21555" windowHeight="10530" tabRatio="730" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21555" windowHeight="10530" tabRatio="730"/>
   </bookViews>
   <sheets>
     <sheet name="Clarinet Arcs" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,21 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Since 0.7
+Enter valid filename. The converter will use as output filename and VST Expression Map name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,6 +68,21 @@
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Since 0.7
+Enter valid filename. The converter will use as output filename and VST Expression Map name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
@@ -75,6 +105,21 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Since 0.7
+Enter valid filename. The converter will use as output filename and VST Expression Map name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,6 +148,21 @@
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Since 0.7
+Enter valid filename. The converter will use as output filename and VST Expression Map name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
@@ -128,6 +188,21 @@
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Since 0.7
+Enter valid filename. The converter will use as output filename and VST Expression Map name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
@@ -144,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="180">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -687,13 +762,31 @@
   </si>
   <si>
     <t>HEAVY VIBRATO</t>
+  </si>
+  <si>
+    <t>Expression Map Name</t>
+  </si>
+  <si>
+    <t>Clarinet Leg Slow</t>
+  </si>
+  <si>
+    <t>Clarinet Arcs</t>
+  </si>
+  <si>
+    <t>Clarinet Bonus FX Runs</t>
+  </si>
+  <si>
+    <t>Clarinet General Arts</t>
+  </si>
+  <si>
+    <t>Clarinet Leg Fast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,8 +833,15 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,6 +887,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,7 +950,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -910,6 +1016,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1212,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -1233,95 +1345,56 @@
     <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6">
-        <v>120</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>166</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -1329,25 +1402,21 @@
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6">
-        <v>120</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -1356,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="6">
         <v>120</v>
@@ -1367,13 +1436,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1382,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6">
         <v>120</v>
@@ -1393,13 +1462,13 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -1408,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6">
         <v>120</v>
@@ -1418,14 +1487,14 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>170</v>
+      <c r="A8" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>170</v>
+      <c r="C8" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -1434,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6">
         <v>120</v>
@@ -1444,14 +1513,14 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
-        <v>171</v>
+      <c r="A9" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>171</v>
+      <c r="C9" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -1460,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6">
         <v>120</v>
@@ -1470,25 +1539,53 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="6">
+        <v>120</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="6">
+        <v>120</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="3"/>
@@ -1496,7 +1593,7 @@
     <row r="12" spans="1:10">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="18"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="6"/>
       <c r="F12" s="2"/>
@@ -1508,7 +1605,7 @@
     <row r="13" spans="1:10">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="18"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="6"/>
       <c r="F13" s="2"/>
@@ -2897,17 +2994,44 @@
       <c r="I128" s="6"/>
       <c r="J128" s="3"/>
     </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="3"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="3"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="3"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B130">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G4:G130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -2922,19 +3046,19 @@
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F128</xm:sqref>
+          <xm:sqref>F4:F130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D128</xm:sqref>
+          <xm:sqref>D4:D130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E128</xm:sqref>
+          <xm:sqref>E4:E130</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2944,13 +3068,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2965,95 +3089,56 @@
     <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6">
-        <v>120</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>146</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -3061,25 +3146,21 @@
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6">
-        <v>120</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -3088,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="6">
         <v>120</v>
@@ -3099,13 +3180,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -3114,7 +3195,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6">
         <v>120</v>
@@ -3125,13 +3206,13 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="17" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -3140,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6">
         <v>120</v>
@@ -3150,14 +3231,14 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>150</v>
+      <c r="A8" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>150</v>
+      <c r="C8" s="17" t="s">
+        <v>148</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -3166,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6">
         <v>120</v>
@@ -3176,25 +3257,53 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="6">
+        <v>120</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="6">
+        <v>120</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="3"/>
@@ -3214,7 +3323,7 @@
     <row r="12" spans="1:10">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="18"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="6"/>
       <c r="F12" s="2"/>
@@ -3226,7 +3335,7 @@
     <row r="13" spans="1:10">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="18"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="6"/>
       <c r="F13" s="2"/>
@@ -4615,18 +4724,45 @@
       <c r="I128" s="6"/>
       <c r="J128" s="3"/>
     </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="3"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="3"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="3"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G4:G130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B130">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4640,19 +4776,19 @@
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E128</xm:sqref>
+          <xm:sqref>E4:E130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D128</xm:sqref>
+          <xm:sqref>D4:D130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Choose from Drop-down list" prompt="If don’t use MIDI Note, set Cell value empty">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F128</xm:sqref>
+          <xm:sqref>F4:F130</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4662,13 +4798,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4683,95 +4819,56 @@
     <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6">
-        <v>120</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>152</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -4779,25 +4876,21 @@
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6">
-        <v>120</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="17" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -4806,7 +4899,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="6">
         <v>120</v>
@@ -4817,13 +4910,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -4832,7 +4925,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6">
         <v>120</v>
@@ -4842,14 +4935,14 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="3" t="s">
-        <v>155</v>
+      <c r="A7" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>155</v>
+      <c r="C7" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -4858,7 +4951,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6">
         <v>120</v>
@@ -4868,25 +4961,53 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="6"/>
+      <c r="A8" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="6">
+        <v>120</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="6"/>
+      <c r="A9" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="6">
+        <v>120</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="3"/>
@@ -4906,7 +5027,7 @@
     <row r="11" spans="1:10">
       <c r="A11" s="3"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="18"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="6"/>
       <c r="F11" s="2"/>
@@ -4918,7 +5039,7 @@
     <row r="12" spans="1:10">
       <c r="A12" s="3"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="18"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="6"/>
       <c r="F12" s="2"/>
@@ -6307,17 +6428,44 @@
       <c r="I127" s="6"/>
       <c r="J127" s="3"/>
     </row>
+    <row r="128" spans="1:10">
+      <c r="A128" s="3"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="18"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+      <c r="J128" s="3"/>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="3"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B127">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B129">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I127">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I129">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G127">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G4:G129">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -6332,19 +6480,19 @@
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F127</xm:sqref>
+          <xm:sqref>F4:F129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D127</xm:sqref>
+          <xm:sqref>D4:D129</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E127</xm:sqref>
+          <xm:sqref>E4:E129</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6354,13 +6502,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6375,95 +6523,56 @@
     <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6">
-        <v>120</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>164</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -6471,25 +6580,21 @@
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6">
-        <v>120</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -6498,7 +6603,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="6">
         <v>120</v>
@@ -6509,13 +6614,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -6524,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6">
         <v>120</v>
@@ -6535,13 +6640,13 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="17" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -6550,7 +6655,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6">
         <v>120</v>
@@ -6560,14 +6665,14 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>173</v>
+      <c r="A8" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>173</v>
+      <c r="C8" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -6576,7 +6681,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6">
         <v>120</v>
@@ -6586,14 +6691,14 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
-        <v>151</v>
+      <c r="A9" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>151</v>
+      <c r="C9" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -6602,7 +6707,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6">
         <v>120</v>
@@ -6613,13 +6718,13 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
@@ -6628,7 +6733,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6">
         <v>120</v>
@@ -6638,25 +6743,53 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="6">
+        <v>120</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="6">
+        <v>120</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="3"/>
@@ -6664,7 +6797,7 @@
     <row r="13" spans="1:10">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="18"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="6"/>
       <c r="F13" s="2"/>
@@ -8053,18 +8186,45 @@
       <c r="I128" s="6"/>
       <c r="J128" s="3"/>
     </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="3"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="3"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="3"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="3">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G4:G130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B130">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8078,19 +8238,19 @@
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E128</xm:sqref>
+          <xm:sqref>E4:E130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D128</xm:sqref>
+          <xm:sqref>D4:D130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Choose from Drop-down list" prompt="If don’t use MIDI Note, set Cell value empty">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F128</xm:sqref>
+          <xm:sqref>F4:F130</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8100,13 +8260,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -8121,95 +8281,56 @@
     <col min="10" max="10" width="50.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="30" customHeight="1">
+      <c r="A1" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E3" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>143</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6">
-        <v>120</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>164</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
@@ -8217,25 +8338,21 @@
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="6">
-        <v>120</v>
-      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -8244,7 +8361,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" s="6">
         <v>120</v>
@@ -8255,13 +8372,13 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -8270,7 +8387,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6">
         <v>120</v>
@@ -8281,13 +8398,13 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="17" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>11</v>
@@ -8296,7 +8413,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6">
         <v>120</v>
@@ -8306,14 +8423,14 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="3" t="s">
-        <v>173</v>
+      <c r="A8" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>173</v>
+      <c r="C8" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
@@ -8322,7 +8439,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6">
         <v>120</v>
@@ -8332,14 +8449,14 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="3" t="s">
-        <v>151</v>
+      <c r="A9" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>151</v>
+      <c r="C9" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -8348,7 +8465,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="6">
         <v>120</v>
@@ -8359,13 +8476,13 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>11</v>
@@ -8374,7 +8491,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6">
         <v>120</v>
@@ -8384,25 +8501,53 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="6">
+        <v>120</v>
+      </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="3"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="6">
+        <v>120</v>
+      </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="3"/>
@@ -8410,7 +8555,7 @@
     <row r="13" spans="1:10">
       <c r="A13" s="3"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="18"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="6"/>
       <c r="F13" s="2"/>
@@ -9799,17 +9944,44 @@
       <c r="I128" s="6"/>
       <c r="J128" s="3"/>
     </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="3"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="6"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="6"/>
+      <c r="H129" s="6"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="3"/>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="3"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="6"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="6"/>
+      <c r="H130" s="6"/>
+      <c r="I130" s="6"/>
+      <c r="J130" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B130">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G2:G128">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty" sqref="G4:G130">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
@@ -9824,19 +9996,19 @@
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$A$2:$A$130</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F128</xm:sqref>
+          <xm:sqref>F4:F130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D128</xm:sqref>
+          <xm:sqref>D4:D130</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E128</xm:sqref>
+          <xm:sqref>E4:E130</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>